<commit_message>
Add date dimension table Minor adjustments to a few code tables in spreadsheet
</commit_message>
<xml_diff>
--- a/analytics/R/r-load/nibrs/inst/raw/NIBRSCodeTables.xlsx
+++ b/analytics/R/r-load/nibrs/inst/raw/NIBRSCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="30525" yWindow="465" windowWidth="24720" windowHeight="14355" tabRatio="705" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="30525" yWindow="465" windowWidth="24720" windowHeight="14355" tabRatio="705" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="636">
   <si>
     <t>Table</t>
   </si>
@@ -1949,6 +1949,12 @@
   </si>
   <si>
     <t>Victim Was Stepsibling</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>98</t>
   </si>
 </sst>
 </file>
@@ -3928,10 +3934,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4147,6 +4153,17 @@
       </c>
       <c r="C19" t="s">
         <v>618</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>98</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="C20" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -5094,10 +5111,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5312,6 +5329,17 @@
       </c>
       <c r="C19" t="s">
         <v>277</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>98</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="C20" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -5443,7 +5471,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5569,13 +5597,16 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="40.125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -5872,6 +5903,17 @@
       </c>
       <c r="C27" t="s">
         <v>463</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>98</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="C28" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -8499,7 +8541,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add materialized view support
</commit_message>
<xml_diff>
--- a/analytics/R/r-load/nibrs/inst/raw/NIBRSCodeTables.xlsx
+++ b/analytics/R/r-load/nibrs/inst/raw/NIBRSCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="30525" yWindow="465" windowWidth="24720" windowHeight="14355" tabRatio="705" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="30525" yWindow="465" windowWidth="24720" windowHeight="14355" tabRatio="705" firstSheet="8" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="636">
   <si>
     <t>Table</t>
   </si>
@@ -3154,10 +3154,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3924,6 +3924,17 @@
       </c>
       <c r="C69" t="s">
         <v>277</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>98</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="C70" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -4174,10 +4185,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4326,6 +4337,17 @@
       </c>
       <c r="C13" t="s">
         <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>98</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="C14" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -8702,7 +8724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>

</xml_diff>